<commit_message>
compared evidencemap stuylist and extracted data and corrected wrong studynames
</commit_message>
<xml_diff>
--- a/02_data/cleandata/df_studylist_cohort.xlsx
+++ b/02_data/cleandata/df_studylist_cohort.xlsx
@@ -1412,13 +1412,13 @@
     <t xml:space="preserve">Focking (2016)</t>
   </si>
   <si>
-    <t xml:space="preserve">Focking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">focking_2016_chr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">focking_2016</t>
+    <t xml:space="preserve">Foecking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foecking_2016_chr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foecking_2016</t>
   </si>
   <si>
     <t xml:space="preserve">Labad (2015)</t>
@@ -3209,16 +3209,16 @@
     <t xml:space="preserve">Oullette-Plamondon (2017)</t>
   </si>
   <si>
-    <t xml:space="preserve">Oullette-Plamondon</t>
+    <t xml:space="preserve">Oullett-Plamondon</t>
   </si>
   <si>
     <t xml:space="preserve">0.9</t>
   </si>
   <si>
-    <t xml:space="preserve">oullette-plamondon_2017_p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oullette-plamondon_2017</t>
+    <t xml:space="preserve">oullett-plamondon_2017_p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oullett-plamondon_2017</t>
   </si>
   <si>
     <t xml:space="preserve">Schimmelmann (2011)</t>

</xml_diff>